<commit_message>
Laget funksjoner for å justere sengekapasitet og antall OR
</commit_message>
<xml_diff>
--- a/input_output/model_input_25groups.xlsx
+++ b/input_output/model_input_25groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oyvindasplin/Documents/Indok/NTNU/Optimering/Master V22/master2022/input_output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erlendcorneliussen/Documents/Studier/Master/GitHub Repository/master2022/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E52D1D2-0210-E14B-BAC1-1D77BDB757DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABC3AF0-0B8C-344C-B77E-9363AEC8A3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21600" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
   <dimension ref="A1:DA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="BT7" sqref="BT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="BT5" s="62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BU5" s="61"/>
       <c r="BV5" s="8">
@@ -3045,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="BT6" s="50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BU6" s="61"/>
       <c r="BV6" s="8">
@@ -18356,7 +18356,7 @@
         <v>3</v>
       </c>
       <c r="I127">
-        <f t="shared" ref="I127:L130" si="21">$E$126</f>
+        <f t="shared" ref="I127:K130" si="21">$E$126</f>
         <v>3</v>
       </c>
       <c r="J127">
@@ -26194,21 +26194,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010014502AD36FC4D1459EE8BFEB917118AE" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b4cd19ef6f825a6ac181b2aef79b604">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1a062c2-eeb0-45d1-8c80-71eb2bb91349" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="944c6668d3530cb8510fee0a023b67da" ns2:_="">
     <xsd:import namespace="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
@@ -26380,10 +26365,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26405,19 +26415,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Laget script for å teste hvor my vi bør øke demand ved 25 surgery groups
</commit_message>
<xml_diff>
--- a/input_output/model_input_25groups.xlsx
+++ b/input_output/model_input_25groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erlendcorneliussen/Documents/Studier/Master/GitHub Repository/master2022/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABC3AF0-0B8C-344C-B77E-9363AEC8A3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02695F78-0AE9-F24E-B419-06DA0BF7964A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21600" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="25720" yWindow="0" windowWidth="25480" windowHeight="28800" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
   <dimension ref="A1:DA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="BT7" sqref="BT7"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AW46" sqref="AW46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26194,6 +26194,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010014502AD36FC4D1459EE8BFEB917118AE" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b4cd19ef6f825a6ac181b2aef79b604">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1a062c2-eeb0-45d1-8c80-71eb2bb91349" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="944c6668d3530cb8510fee0a023b67da" ns2:_="">
     <xsd:import namespace="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
@@ -26365,12 +26371,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -26381,6 +26381,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26398,22 +26414,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Oppdatert excel-fil for 25 groups
</commit_message>
<xml_diff>
--- a/input_output/model_input_25groups.xlsx
+++ b/input_output/model_input_25groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sambaad.stud.ntnu.no\oyviasp\.profil\stud\datasal\Desktop\master2022\input_output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erlendcorneliussen/Documents/Studier/NTNU/2022 vaar/Master/master2022/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8A17A0-7786-4757-A06D-2E74A87DC581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5842EE3-40FE-AD45-B8F6-CF92A8C5C095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29100" windowHeight="8325" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -953,7 +953,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1380,7 +1380,7 @@
     <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{8F977E11-39D4-E04C-8D51-A4F1FE1B59AD}"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1694,29 +1694,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
   <dimension ref="A1:DA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:AJ3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AO25" sqref="AO25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="6" width="10.125" customWidth="1"/>
-    <col min="7" max="7" width="2.875" customWidth="1"/>
-    <col min="9" max="36" width="4.625" customWidth="1"/>
+    <col min="2" max="6" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+    <col min="9" max="36" width="4.6640625" customWidth="1"/>
     <col min="37" max="37" width="7" customWidth="1"/>
     <col min="38" max="38" width="4.5" customWidth="1"/>
-    <col min="39" max="39" width="11.125" customWidth="1"/>
-    <col min="40" max="40" width="12.625" customWidth="1"/>
-    <col min="41" max="41" width="13.125" customWidth="1"/>
+    <col min="39" max="39" width="11.1640625" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" customWidth="1"/>
+    <col min="41" max="41" width="13.1640625" customWidth="1"/>
     <col min="42" max="42" width="3.5" customWidth="1"/>
-    <col min="43" max="43" width="8.875" customWidth="1"/>
+    <col min="43" max="43" width="8.83203125" customWidth="1"/>
     <col min="44" max="71" width="3.5" customWidth="1"/>
-    <col min="72" max="72" width="10.875" customWidth="1"/>
-    <col min="74" max="74" width="4.375" customWidth="1"/>
-    <col min="78" max="105" width="8.875" customWidth="1"/>
+    <col min="72" max="72" width="10.83203125" customWidth="1"/>
+    <col min="74" max="74" width="4.33203125" customWidth="1"/>
+    <col min="78" max="105" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105" s="3" customFormat="1" ht="16.5" thickBot="1">
+    <row r="1" spans="1:105" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="21" t="s">
         <v>181</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:105" ht="16.5" thickBot="1">
+    <row r="2" spans="1:105" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="31">
         <v>0.1</v>
@@ -2135,7 +2135,7 @@
         <v>64</v>
       </c>
       <c r="AO2" s="49">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="AP2" s="61"/>
       <c r="AQ2" s="25" t="s">
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:105" ht="16.5" thickBot="1">
+    <row r="3" spans="1:105" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
@@ -2430,7 +2430,7 @@
         <v>272.5</v>
       </c>
       <c r="AO3" s="62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AP3" s="61"/>
       <c r="AQ3" s="25" t="s">
@@ -2619,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:105">
+    <row r="4" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="61"/>
       <c r="C4" s="61"/>
@@ -2665,7 +2665,7 @@
         <v>348.5</v>
       </c>
       <c r="AO4" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP4" s="61"/>
       <c r="AQ4" s="25" t="s">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="BX4" s="2"/>
     </row>
-    <row r="5" spans="1:105">
+    <row r="5" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="61"/>
       <c r="C5" s="61"/>
@@ -2813,7 +2813,7 @@
         <v>352</v>
       </c>
       <c r="AO5" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP5" s="61"/>
       <c r="AQ5" s="25" t="s">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="BX5" s="2"/>
     </row>
-    <row r="6" spans="1:105" ht="16.5" thickBot="1">
+    <row r="6" spans="1:105" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="61"/>
       <c r="C6" s="61"/>
@@ -2961,7 +2961,7 @@
         <v>208</v>
       </c>
       <c r="AO6" s="62">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AP6" s="61"/>
       <c r="AQ6" s="25" t="s">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="BX6" s="2"/>
     </row>
-    <row r="7" spans="1:105">
+    <row r="7" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="61"/>
       <c r="C7" s="61"/>
@@ -3109,7 +3109,7 @@
         <v>397</v>
       </c>
       <c r="AO7" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP7" s="61"/>
       <c r="AQ7" s="61"/>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="BX7" s="2"/>
     </row>
-    <row r="8" spans="1:105">
+    <row r="8" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="61"/>
       <c r="C8" s="61"/>
@@ -3197,7 +3197,7 @@
         <v>67</v>
       </c>
       <c r="AO8" s="62">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AP8" s="61"/>
       <c r="AQ8" s="61"/>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="BX8" s="2"/>
     </row>
-    <row r="9" spans="1:105">
+    <row r="9" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="61"/>
       <c r="C9" s="61"/>
@@ -3285,7 +3285,7 @@
         <v>211</v>
       </c>
       <c r="AO9" s="62">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="AP9" s="61"/>
       <c r="AQ9" s="61"/>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="BX9" s="2"/>
     </row>
-    <row r="10" spans="1:105">
+    <row r="10" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="61"/>
       <c r="C10" s="61"/>
@@ -3373,7 +3373,7 @@
         <v>188.5</v>
       </c>
       <c r="AO10" s="62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AP10" s="61"/>
       <c r="AQ10" s="61"/>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="BX10" s="2"/>
     </row>
-    <row r="11" spans="1:105">
+    <row r="11" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
@@ -3461,7 +3461,7 @@
         <v>425</v>
       </c>
       <c r="AO11" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP11" s="61"/>
       <c r="AQ11" s="61"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="BX11" s="2"/>
     </row>
-    <row r="12" spans="1:105">
+    <row r="12" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
@@ -3549,7 +3549,7 @@
         <v>235</v>
       </c>
       <c r="AO12" s="62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AP12" s="61"/>
       <c r="AQ12" s="61"/>
@@ -3591,7 +3591,7 @@
       </c>
       <c r="BX12" s="2"/>
     </row>
-    <row r="13" spans="1:105">
+    <row r="13" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="61"/>
       <c r="C13" s="61"/>
@@ -3637,7 +3637,7 @@
         <v>272</v>
       </c>
       <c r="AO13" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP13" s="61"/>
       <c r="AQ13" s="61"/>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="BX13" s="2"/>
     </row>
-    <row r="14" spans="1:105">
+    <row r="14" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="61"/>
       <c r="C14" s="61"/>
@@ -3725,7 +3725,7 @@
         <v>226</v>
       </c>
       <c r="AO14" s="62">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AP14" s="61"/>
       <c r="AQ14" s="61"/>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="BX14" s="2"/>
     </row>
-    <row r="15" spans="1:105">
+    <row r="15" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -3813,7 +3813,7 @@
         <v>210</v>
       </c>
       <c r="AO15" s="62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AP15" s="61"/>
       <c r="AQ15" s="61"/>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="BX15" s="2"/>
     </row>
-    <row r="16" spans="1:105">
+    <row r="16" spans="1:105" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="61"/>
       <c r="C16" s="61"/>
@@ -3901,7 +3901,7 @@
         <v>61.5</v>
       </c>
       <c r="AO16" s="62">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="AP16" s="61"/>
       <c r="AQ16" s="61"/>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="BX16" s="2"/>
     </row>
-    <row r="17" spans="1:76">
+    <row r="17" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="61"/>
       <c r="C17" s="61"/>
@@ -3989,7 +3989,7 @@
         <v>211</v>
       </c>
       <c r="AO17" s="62">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AP17" s="61"/>
       <c r="AQ17" s="61"/>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="BX17" s="2"/>
     </row>
-    <row r="18" spans="1:76">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="61"/>
       <c r="C18" s="61"/>
@@ -4077,7 +4077,7 @@
         <v>106</v>
       </c>
       <c r="AO18" s="62">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="AP18" s="61"/>
       <c r="AQ18" s="61"/>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="BX18" s="2"/>
     </row>
-    <row r="19" spans="1:76">
+    <row r="19" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="61"/>
       <c r="C19" s="61"/>
@@ -4165,7 +4165,7 @@
         <v>305</v>
       </c>
       <c r="AO19" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP19" s="61"/>
       <c r="AQ19" s="61"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="BX19" s="2"/>
     </row>
-    <row r="20" spans="1:76">
+    <row r="20" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="61"/>
       <c r="C20" s="61"/>
@@ -4253,7 +4253,7 @@
         <v>52.5</v>
       </c>
       <c r="AO20" s="62">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AP20" s="61"/>
       <c r="AQ20" s="61"/>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="BX20" s="2"/>
     </row>
-    <row r="21" spans="1:76">
+    <row r="21" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="61"/>
       <c r="C21" s="61"/>
@@ -4341,7 +4341,7 @@
         <v>106</v>
       </c>
       <c r="AO21" s="62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AP21" s="61"/>
       <c r="AQ21" s="61"/>
@@ -4383,7 +4383,7 @@
       </c>
       <c r="BX21" s="2"/>
     </row>
-    <row r="22" spans="1:76">
+    <row r="22" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="61"/>
       <c r="C22" s="61"/>
@@ -4429,7 +4429,7 @@
         <v>142</v>
       </c>
       <c r="AO22" s="62">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="AP22" s="61"/>
       <c r="AQ22" s="61"/>
@@ -4471,7 +4471,7 @@
       </c>
       <c r="BX22" s="2"/>
     </row>
-    <row r="23" spans="1:76">
+    <row r="23" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="61"/>
       <c r="C23" s="61"/>
@@ -4517,7 +4517,7 @@
         <v>134</v>
       </c>
       <c r="AO23" s="62">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AP23" s="61"/>
       <c r="AQ23" s="61"/>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="BX23" s="2"/>
     </row>
-    <row r="24" spans="1:76">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="61"/>
       <c r="C24" s="61"/>
@@ -4605,7 +4605,7 @@
         <v>86</v>
       </c>
       <c r="AO24" s="62">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="AP24" s="61"/>
       <c r="AQ24" s="61"/>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="BX24" s="2"/>
     </row>
-    <row r="25" spans="1:76">
+    <row r="25" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="61"/>
       <c r="C25" s="61"/>
@@ -4693,7 +4693,7 @@
         <v>187</v>
       </c>
       <c r="AO25" s="62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AP25" s="61"/>
       <c r="AQ25" s="61"/>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="BX25" s="2"/>
     </row>
-    <row r="26" spans="1:76" ht="16.5" thickBot="1">
+    <row r="26" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="61"/>
       <c r="C26" s="61"/>
@@ -4781,7 +4781,7 @@
         <v>225.5</v>
       </c>
       <c r="AO26" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AP26" s="61"/>
       <c r="AQ26" s="61"/>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="BX26" s="2"/>
     </row>
-    <row r="27" spans="1:76">
+    <row r="27" spans="1:76" x14ac:dyDescent="0.2">
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
@@ -4903,7 +4903,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="28" spans="1:76">
+    <row r="28" spans="1:76" x14ac:dyDescent="0.2">
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -4983,7 +4983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:76" ht="16.5" thickBot="1">
+    <row r="29" spans="1:76" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AT29" s="61"/>
       <c r="AU29" s="61"/>
       <c r="AV29" s="61"/>
@@ -4994,92 +4994,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:76">
+    <row r="30" spans="1:76" x14ac:dyDescent="0.2">
       <c r="AT30" s="61"/>
       <c r="AU30" s="61"/>
       <c r="AV30" s="61"/>
     </row>
-    <row r="31" spans="1:76">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.2">
       <c r="AT31" s="61"/>
       <c r="AU31" s="61"/>
       <c r="AV31" s="61"/>
     </row>
-    <row r="32" spans="1:76">
+    <row r="32" spans="1:76" x14ac:dyDescent="0.2">
       <c r="AT32" s="61"/>
       <c r="AU32" s="61"/>
       <c r="AV32" s="61"/>
     </row>
-    <row r="33" spans="46:48">
+    <row r="33" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT33" s="61"/>
       <c r="AU33" s="61"/>
       <c r="AV33" s="61"/>
     </row>
-    <row r="34" spans="46:48">
+    <row r="34" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT34" s="61"/>
       <c r="AU34" s="61"/>
       <c r="AV34" s="61"/>
     </row>
-    <row r="35" spans="46:48">
+    <row r="35" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT35" s="61"/>
       <c r="AU35" s="61"/>
       <c r="AV35" s="61"/>
     </row>
-    <row r="36" spans="46:48">
+    <row r="36" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT36" s="61"/>
       <c r="AU36" s="61"/>
       <c r="AV36" s="61"/>
     </row>
-    <row r="37" spans="46:48">
+    <row r="37" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT37" s="61"/>
       <c r="AU37" s="61"/>
       <c r="AV37" s="61"/>
     </row>
-    <row r="38" spans="46:48">
+    <row r="38" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT38" s="61"/>
       <c r="AU38" s="61"/>
       <c r="AV38" s="61"/>
     </row>
-    <row r="39" spans="46:48">
+    <row r="39" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT39" s="61"/>
       <c r="AU39" s="61"/>
       <c r="AV39" s="61"/>
     </row>
-    <row r="40" spans="46:48">
+    <row r="40" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT40" s="61"/>
       <c r="AU40" s="61"/>
       <c r="AV40" s="61"/>
     </row>
-    <row r="41" spans="46:48">
+    <row r="41" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT41" s="61"/>
       <c r="AU41" s="61"/>
       <c r="AV41" s="61"/>
     </row>
-    <row r="42" spans="46:48">
+    <row r="42" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT42" s="61"/>
       <c r="AU42" s="61"/>
       <c r="AV42" s="61"/>
     </row>
-    <row r="43" spans="46:48">
+    <row r="43" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT43" s="61"/>
       <c r="AU43" s="61"/>
       <c r="AV43" s="61"/>
     </row>
-    <row r="44" spans="46:48">
+    <row r="44" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT44" s="61"/>
       <c r="AU44" s="61"/>
       <c r="AV44" s="61"/>
     </row>
-    <row r="45" spans="46:48">
+    <row r="45" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT45" s="61"/>
       <c r="AU45" s="61"/>
       <c r="AV45" s="61"/>
     </row>
-    <row r="46" spans="46:48">
+    <row r="46" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT46" s="61"/>
       <c r="AU46" s="61"/>
       <c r="AV46" s="61"/>
     </row>
-    <row r="47" spans="46:48">
+    <row r="47" spans="46:48" x14ac:dyDescent="0.2">
       <c r="AT47" s="61"/>
       <c r="AU47" s="61"/>
       <c r="AV47" s="61"/>
@@ -5097,22 +5097,22 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="5.125" customWidth="1"/>
-    <col min="4" max="4" width="12.125" customWidth="1"/>
-    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" customWidth="1"/>
     <col min="7" max="31" width="4" customWidth="1"/>
-    <col min="32" max="32" width="4.375" customWidth="1"/>
-    <col min="34" max="58" width="5.125" customWidth="1"/>
-    <col min="59" max="65" width="3.875" customWidth="1"/>
-    <col min="66" max="66" width="4.625" customWidth="1"/>
+    <col min="32" max="32" width="4.33203125" customWidth="1"/>
+    <col min="34" max="58" width="5.1640625" customWidth="1"/>
+    <col min="59" max="65" width="3.83203125" customWidth="1"/>
+    <col min="66" max="66" width="4.6640625" customWidth="1"/>
     <col min="67" max="67" width="6" customWidth="1"/>
-    <col min="68" max="68" width="4.375" customWidth="1"/>
+    <col min="68" max="68" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:77" ht="16.5" thickBot="1">
+    <row r="1" spans="2:77" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>180</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="2:77">
+    <row r="2" spans="2:77" x14ac:dyDescent="0.2">
       <c r="B2" s="32" t="s">
         <v>2</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:77" ht="16.5" thickBot="1">
+    <row r="3" spans="2:77" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="39" t="s">
         <v>5</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:77">
+    <row r="4" spans="2:77" x14ac:dyDescent="0.2">
       <c r="B4" s="39" t="s">
         <v>8</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:77">
+    <row r="5" spans="2:77" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:77" ht="16.5" thickBot="1">
+    <row r="6" spans="2:77" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
         <v>9</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:77">
+    <row r="7" spans="2:77" x14ac:dyDescent="0.2">
       <c r="B7" s="39" t="s">
         <v>12</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="2:77" ht="16.5" thickBot="1">
+    <row r="8" spans="2:77" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
@@ -6016,92 +6016,92 @@
       <c r="BX8" s="44"/>
       <c r="BY8" s="44"/>
     </row>
-    <row r="9" spans="2:77">
+    <row r="9" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D9" s="46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:77">
+    <row r="10" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D10" s="47" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="2:77">
+    <row r="11" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D11" s="47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:77">
+    <row r="12" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D12" s="47" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="2:77">
+    <row r="13" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D13" s="47" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="2:77">
+    <row r="14" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D14" s="47" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:77">
+    <row r="15" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D15" s="47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:77">
+    <row r="16" spans="2:77" x14ac:dyDescent="0.2">
       <c r="D16" s="47" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="47" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D18" s="47" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" s="47" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" s="47" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" s="47" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D22" s="47" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D23" s="47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D24" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" s="47" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="4:4" ht="16.5" thickBot="1">
+    <row r="26" spans="4:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D26" s="48" t="s">
         <v>116</v>
       </c>
@@ -6120,9 +6120,9 @@
       <selection activeCell="A32" sqref="A32:BE102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" thickBot="1">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>111</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>108</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>110</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>5.1020408163265302E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>109</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>114</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>113</v>
       </c>
@@ -6837,7 +6837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>112</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>5.4054054054054057E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>107</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>103</v>
       </c>
@@ -7227,7 +7227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>104</v>
       </c>
@@ -7292,7 +7292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>105</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>3.8461538461538464E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>118</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>117</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="16.5" thickBot="1">
+    <row r="26" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
@@ -7836,7 +7836,7 @@
       <c r="AP27" s="4"/>
       <c r="AQ27" s="4"/>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
@@ -7860,7 +7860,7 @@
       <c r="AP28" s="4"/>
       <c r="AQ28" s="4"/>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -7883,7 +7883,7 @@
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -7906,7 +7906,7 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -7929,7 +7929,7 @@
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -7952,7 +7952,7 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -7975,7 +7975,7 @@
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -7998,7 +7998,7 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -8021,7 +8021,7 @@
       <c r="T45" s="4"/>
       <c r="U45" s="4"/>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -8044,7 +8044,7 @@
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -8067,7 +8067,7 @@
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
     </row>
-    <row r="51" spans="1:21">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -8090,7 +8090,7 @@
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -8113,7 +8113,7 @@
       <c r="T53" s="4"/>
       <c r="U53" s="4"/>
     </row>
-    <row r="55" spans="1:21">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -8136,7 +8136,7 @@
       <c r="T55" s="4"/>
       <c r="U55" s="4"/>
     </row>
-    <row r="57" spans="1:21">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -8159,7 +8159,7 @@
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="59" spans="1:21">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -8182,7 +8182,7 @@
       <c r="T59" s="4"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -8205,7 +8205,7 @@
       <c r="T61" s="4"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="63" spans="1:21">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -8228,7 +8228,7 @@
       <c r="T63" s="4"/>
       <c r="U63" s="4"/>
     </row>
-    <row r="65" spans="1:21">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -8251,7 +8251,7 @@
       <c r="T65" s="4"/>
       <c r="U65" s="4"/>
     </row>
-    <row r="67" spans="1:21">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -8274,7 +8274,7 @@
       <c r="T67" s="4"/>
       <c r="U67" s="4"/>
     </row>
-    <row r="69" spans="1:21">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -8297,7 +8297,7 @@
       <c r="T69" s="4"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="71" spans="1:21">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -8320,7 +8320,7 @@
       <c r="T71" s="4"/>
       <c r="U71" s="4"/>
     </row>
-    <row r="73" spans="1:21">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -8343,7 +8343,7 @@
       <c r="T73" s="4"/>
       <c r="U73" s="4"/>
     </row>
-    <row r="75" spans="1:21">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -8366,7 +8366,7 @@
       <c r="T75" s="4"/>
       <c r="U75" s="4"/>
     </row>
-    <row r="77" spans="1:21">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -8389,7 +8389,7 @@
       <c r="T77" s="4"/>
       <c r="U77" s="4"/>
     </row>
-    <row r="79" spans="1:21">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -8412,7 +8412,7 @@
       <c r="T79" s="4"/>
       <c r="U79" s="4"/>
     </row>
-    <row r="81" spans="1:21">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -8435,7 +8435,7 @@
       <c r="T81" s="4"/>
       <c r="U81" s="4"/>
     </row>
-    <row r="83" spans="1:21">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -8458,7 +8458,7 @@
       <c r="T83" s="4"/>
       <c r="U83" s="4"/>
     </row>
-    <row r="85" spans="1:21">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -8481,7 +8481,7 @@
       <c r="T85" s="4"/>
       <c r="U85" s="4"/>
     </row>
-    <row r="87" spans="1:21">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -8504,7 +8504,7 @@
       <c r="T87" s="4"/>
       <c r="U87" s="4"/>
     </row>
-    <row r="89" spans="1:21">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -8527,7 +8527,7 @@
       <c r="T89" s="4"/>
       <c r="U89" s="4"/>
     </row>
-    <row r="91" spans="1:21">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -8550,7 +8550,7 @@
       <c r="T91" s="4"/>
       <c r="U91" s="4"/>
     </row>
-    <row r="93" spans="1:21">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -8573,7 +8573,7 @@
       <c r="T93" s="4"/>
       <c r="U93" s="4"/>
     </row>
-    <row r="95" spans="1:21">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -8596,7 +8596,7 @@
       <c r="T95" s="4"/>
       <c r="U95" s="4"/>
     </row>
-    <row r="97" spans="1:21">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -8619,7 +8619,7 @@
       <c r="T97" s="4"/>
       <c r="U97" s="4"/>
     </row>
-    <row r="99" spans="1:21">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -8642,7 +8642,7 @@
       <c r="T99" s="4"/>
       <c r="U99" s="4"/>
     </row>
-    <row r="101" spans="1:21">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -8682,9 +8682,9 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:45" ht="16.5" thickBot="1">
+    <row r="1" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
@@ -8772,7 +8772,7 @@
       <c r="AR1" s="5"/>
       <c r="AS1" s="5"/>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -8860,7 +8860,7 @@
       <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -8948,7 +8948,7 @@
       <c r="AR3" s="5"/>
       <c r="AS3" s="5"/>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>111</v>
       </c>
@@ -9036,7 +9036,7 @@
       <c r="AR4" s="5"/>
       <c r="AS4" s="5"/>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>108</v>
       </c>
@@ -9124,7 +9124,7 @@
       <c r="AR5" s="5"/>
       <c r="AS5" s="5"/>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>110</v>
       </c>
@@ -9212,7 +9212,7 @@
       <c r="AR6" s="5"/>
       <c r="AS6" s="5"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>109</v>
       </c>
@@ -9300,7 +9300,7 @@
       <c r="AR7" s="5"/>
       <c r="AS7" s="5"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -9388,7 +9388,7 @@
       <c r="AR8" s="5"/>
       <c r="AS8" s="5"/>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -9476,7 +9476,7 @@
       <c r="AR9" s="5"/>
       <c r="AS9" s="5"/>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>114</v>
       </c>
@@ -9564,7 +9564,7 @@
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>113</v>
       </c>
@@ -9652,7 +9652,7 @@
       <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>112</v>
       </c>
@@ -9740,7 +9740,7 @@
       <c r="AR12" s="5"/>
       <c r="AS12" s="5"/>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -9828,7 +9828,7 @@
       <c r="AR13" s="5"/>
       <c r="AS13" s="5"/>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -9916,7 +9916,7 @@
       <c r="AR14" s="5"/>
       <c r="AS14" s="5"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -10004,7 +10004,7 @@
       <c r="AR15" s="5"/>
       <c r="AS15" s="5"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>107</v>
       </c>
@@ -10092,7 +10092,7 @@
       <c r="AR16" s="5"/>
       <c r="AS16" s="5"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>103</v>
       </c>
@@ -10180,7 +10180,7 @@
       <c r="AR17" s="5"/>
       <c r="AS17" s="5"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>104</v>
       </c>
@@ -10268,7 +10268,7 @@
       <c r="AR18" s="5"/>
       <c r="AS18" s="5"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -10356,7 +10356,7 @@
       <c r="AR19" s="5"/>
       <c r="AS19" s="5"/>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>105</v>
       </c>
@@ -10444,7 +10444,7 @@
       <c r="AR20" s="5"/>
       <c r="AS20" s="5"/>
     </row>
-    <row r="21" spans="1:45">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
@@ -10532,7 +10532,7 @@
       <c r="AR21" s="5"/>
       <c r="AS21" s="5"/>
     </row>
-    <row r="22" spans="1:45">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
@@ -10620,7 +10620,7 @@
       <c r="AR22" s="5"/>
       <c r="AS22" s="5"/>
     </row>
-    <row r="23" spans="1:45">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -10708,7 +10708,7 @@
       <c r="AR23" s="5"/>
       <c r="AS23" s="5"/>
     </row>
-    <row r="24" spans="1:45">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>118</v>
       </c>
@@ -10796,7 +10796,7 @@
       <c r="AR24" s="5"/>
       <c r="AS24" s="5"/>
     </row>
-    <row r="25" spans="1:45">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>117</v>
       </c>
@@ -10884,7 +10884,7 @@
       <c r="AR25" s="5"/>
       <c r="AS25" s="5"/>
     </row>
-    <row r="26" spans="1:45" ht="16.5" thickBot="1">
+    <row r="26" spans="1:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -10972,7 +10972,7 @@
       <c r="AR26" s="5"/>
       <c r="AS26" s="5"/>
     </row>
-    <row r="27" spans="1:45">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
@@ -10990,7 +10990,7 @@
       <c r="AJ27" s="4"/>
       <c r="AK27" s="4"/>
     </row>
-    <row r="28" spans="1:45">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
@@ -11008,7 +11008,7 @@
       <c r="AJ28" s="4"/>
       <c r="AK28" s="4"/>
     </row>
-    <row r="29" spans="1:45">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
@@ -11026,7 +11026,7 @@
       <c r="AJ29" s="4"/>
       <c r="AK29" s="4"/>
     </row>
-    <row r="30" spans="1:45">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
@@ -11044,7 +11044,7 @@
       <c r="AJ30" s="4"/>
       <c r="AK30" s="4"/>
     </row>
-    <row r="31" spans="1:45">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
@@ -11062,7 +11062,7 @@
       <c r="AJ31" s="4"/>
       <c r="AK31" s="4"/>
     </row>
-    <row r="32" spans="1:45">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
@@ -11097,12 +11097,12 @@
       <selection activeCell="H147" sqref="H147:AI148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" thickBot="1">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
@@ -11167,7 +11167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -11297,7 +11297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>111</v>
       </c>
@@ -11362,7 +11362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>108</v>
       </c>
@@ -11427,7 +11427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>110</v>
       </c>
@@ -11492,7 +11492,7 @@
         <v>5.1020408163265302E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>109</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>114</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>113</v>
       </c>
@@ -11817,7 +11817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>112</v>
       </c>
@@ -11882,7 +11882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -11947,7 +11947,7 @@
         <v>5.4054054054054057E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -12012,7 +12012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -12077,7 +12077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>107</v>
       </c>
@@ -12142,7 +12142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>103</v>
       </c>
@@ -12207,7 +12207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>104</v>
       </c>
@@ -12272,7 +12272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>105</v>
       </c>
@@ -12402,7 +12402,7 @@
         <v>3.8461538461538464E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
@@ -12467,7 +12467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
@@ -12532,7 +12532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -12597,7 +12597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>118</v>
       </c>
@@ -12662,7 +12662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>117</v>
       </c>
@@ -12727,7 +12727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="16.5" thickBot="1">
+    <row r="26" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -12792,7 +12792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
@@ -12816,7 +12816,7 @@
       <c r="AP27" s="4"/>
       <c r="AQ27" s="4"/>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
@@ -12840,7 +12840,7 @@
       <c r="AP28" s="4"/>
       <c r="AQ28" s="4"/>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -12863,7 +12863,7 @@
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -12886,7 +12886,7 @@
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -12909,7 +12909,7 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
     </row>
-    <row r="41" spans="1:26" ht="16.5" thickBot="1">
+    <row r="41" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="W41" t="s">
         <v>188</v>
       </c>
@@ -12917,7 +12917,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -13012,7 +13012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -13107,7 +13107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:26">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -13297,7 +13297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -13392,7 +13392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -13487,7 +13487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -13582,7 +13582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:26">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -13677,7 +13677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -13772,7 +13772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:26">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -13867,7 +13867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -13962,7 +13962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:26">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -14057,7 +14057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:26">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -14152,7 +14152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:26">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -14247,7 +14247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:26">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -14342,7 +14342,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:26">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:26">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -14532,7 +14532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:26">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>106</v>
       </c>
@@ -14627,7 +14627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:26">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>105</v>
       </c>
@@ -14722,7 +14722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:26">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>34</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:26">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -14912,7 +14912,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:26">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -15007,7 +15007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:26">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -15102,7 +15102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:60">
+    <row r="65" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -15197,7 +15197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:60" ht="16.5" thickBot="1">
+    <row r="66" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>116</v>
       </c>
@@ -15292,8 +15292,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:60" ht="16.5" thickBot="1"/>
-    <row r="68" spans="1:60" ht="16.5" thickBot="1">
+    <row r="67" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>190</v>
       </c>
@@ -15378,7 +15378,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:60">
+    <row r="71" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>191</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:60">
+    <row r="72" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>1</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:60">
+    <row r="73" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B73">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -15717,7 +15717,7 @@
       </c>
       <c r="AC73" s="69"/>
     </row>
-    <row r="74" spans="1:60">
+    <row r="74" spans="1:60" x14ac:dyDescent="0.2">
       <c r="C74">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -15800,7 +15800,7 @@
       </c>
       <c r="AC74" s="69"/>
     </row>
-    <row r="75" spans="1:60">
+    <row r="75" spans="1:60" x14ac:dyDescent="0.2">
       <c r="D75">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -15883,7 +15883,7 @@
       </c>
       <c r="AC75" s="69"/>
     </row>
-    <row r="76" spans="1:60">
+    <row r="76" spans="1:60" x14ac:dyDescent="0.2">
       <c r="E76">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -15966,7 +15966,7 @@
       </c>
       <c r="AC76" s="69"/>
     </row>
-    <row r="77" spans="1:60">
+    <row r="77" spans="1:60" x14ac:dyDescent="0.2">
       <c r="F77">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16049,7 +16049,7 @@
       </c>
       <c r="AC77" s="69"/>
     </row>
-    <row r="78" spans="1:60">
+    <row r="78" spans="1:60" x14ac:dyDescent="0.2">
       <c r="I78">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16132,7 +16132,7 @@
       </c>
       <c r="AC78" s="69"/>
     </row>
-    <row r="79" spans="1:60">
+    <row r="79" spans="1:60" x14ac:dyDescent="0.2">
       <c r="J79">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16214,7 +16214,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:60">
+    <row r="80" spans="1:60" x14ac:dyDescent="0.2">
       <c r="K80">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16296,7 +16296,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:60">
+    <row r="81" spans="1:60" x14ac:dyDescent="0.2">
       <c r="L81">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16378,7 +16378,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:60">
+    <row r="82" spans="1:60" x14ac:dyDescent="0.2">
       <c r="M82">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16460,7 +16460,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:60">
+    <row r="83" spans="1:60" x14ac:dyDescent="0.2">
       <c r="P83">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16542,7 +16542,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:60">
+    <row r="84" spans="1:60" x14ac:dyDescent="0.2">
       <c r="Q84">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16624,7 +16624,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:60">
+    <row r="85" spans="1:60" x14ac:dyDescent="0.2">
       <c r="R85">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16706,7 +16706,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:60">
+    <row r="86" spans="1:60" x14ac:dyDescent="0.2">
       <c r="S86">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16788,7 +16788,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:60">
+    <row r="87" spans="1:60" x14ac:dyDescent="0.2">
       <c r="T87">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16870,7 +16870,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:60">
+    <row r="88" spans="1:60" x14ac:dyDescent="0.2">
       <c r="W88">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -16952,7 +16952,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:60">
+    <row r="89" spans="1:60" x14ac:dyDescent="0.2">
       <c r="X89">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -17034,7 +17034,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:60">
+    <row r="90" spans="1:60" x14ac:dyDescent="0.2">
       <c r="Y90">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -17116,7 +17116,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:60">
+    <row r="91" spans="1:60" x14ac:dyDescent="0.2">
       <c r="Z91">
         <f>$B$68</f>
         <v>8.4316816207935581</v>
@@ -17198,7 +17198,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:60">
+    <row r="92" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B92" s="73"/>
       <c r="C92" s="73"/>
       <c r="D92" s="73"/>
@@ -17305,7 +17305,7 @@
         <v>1.3717807289235863E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:60" ht="16.5" thickBot="1">
+    <row r="93" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>198</v>
       </c>
@@ -17422,7 +17422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:60" ht="16.5" thickBot="1">
+    <row r="94" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AF94" t="s">
         <v>198</v>
       </c>
@@ -17531,7 +17531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:60">
+    <row r="95" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>281</v>
       </c>
@@ -17648,7 +17648,7 @@
         <v>16.061181057689225</v>
       </c>
     </row>
-    <row r="96" spans="1:60">
+    <row r="96" spans="1:60" x14ac:dyDescent="0.2">
       <c r="AF96" t="s">
         <v>201</v>
       </c>
@@ -17737,7 +17737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:60">
+    <row r="97" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>283</v>
       </c>
@@ -17941,7 +17941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:60">
+    <row r="98" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>282</v>
       </c>
@@ -18033,17 +18033,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:60">
+    <row r="99" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:60">
+    <row r="100" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>24.5</v>
       </c>
     </row>
-    <row r="102" spans="1:60">
+    <row r="102" spans="1:60" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
         <v>285</v>
       </c>
@@ -18054,7 +18054,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="103" spans="1:60">
+    <row r="103" spans="1:60" x14ac:dyDescent="0.2">
       <c r="C103" s="75">
         <f>(SUM(B97:E97)+SUM(I97:L97)+SUM(P97:S97)+SUM(W97:Z97))/(16)</f>
         <v>0.82352703252328951</v>
@@ -18068,7 +18068,7 @@
         <v>0.85328616598666263</v>
       </c>
     </row>
-    <row r="107" spans="1:60">
+    <row r="107" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>290</v>
       </c>
@@ -18085,7 +18085,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="108" spans="1:60">
+    <row r="108" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>288</v>
       </c>
@@ -18105,7 +18105,7 @@
         <v>0.85328616598666263</v>
       </c>
     </row>
-    <row r="109" spans="1:60">
+    <row r="109" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>200</v>
       </c>
@@ -18125,7 +18125,7 @@
         <v>0.85322557172891611</v>
       </c>
     </row>
-    <row r="110" spans="1:60">
+    <row r="110" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>291</v>
       </c>
@@ -18145,17 +18145,17 @@
         <v>0.85348612559247861</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>293</v>
       </c>
@@ -18166,7 +18166,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>33</v>
       </c>
@@ -18205,7 +18205,7 @@
         <v>11.600000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>290</v>
       </c>
@@ -18248,7 +18248,7 @@
         <v>11.600000000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>289</v>
       </c>
@@ -18292,7 +18292,7 @@
         <v>11.600000000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>44</v>
       </c>
@@ -18328,7 +18328,7 @@
         <v>11.600000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>290</v>
       </c>
@@ -18343,7 +18343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>289</v>
       </c>
@@ -18387,7 +18387,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H128">
         <f t="shared" ref="H128:H130" si="23">$E$126</f>
         <v>3</v>
@@ -18417,7 +18417,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H129">
         <f t="shared" si="23"/>
         <v>3</v>
@@ -18447,7 +18447,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="130" spans="1:14">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H130">
         <f t="shared" si="23"/>
         <v>3</v>
@@ -18477,12 +18477,12 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>293</v>
       </c>
@@ -18493,7 +18493,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="136" spans="1:14">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>33</v>
       </c>
@@ -18532,7 +18532,7 @@
         <v>11.100000000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:14">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>290</v>
       </c>
@@ -18575,7 +18575,7 @@
         <v>11.100000000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:14">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>289</v>
       </c>
@@ -18619,7 +18619,7 @@
         <v>11.100000000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:14">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>44</v>
       </c>
@@ -18655,7 +18655,7 @@
         <v>11.100000000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:14">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>290</v>
       </c>
@@ -18677,7 +18677,7 @@
       <c r="M140" s="77"/>
       <c r="N140" s="77"/>
     </row>
-    <row r="141" spans="1:14">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>289</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="142" spans="1:14">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H142" s="77">
         <f t="shared" ref="H142:H144" si="31">$E$140</f>
         <v>2.7</v>
@@ -18751,7 +18751,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="143" spans="1:14">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H143" s="77">
         <f t="shared" si="31"/>
         <v>2.7</v>
@@ -18781,7 +18781,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="144" spans="1:14">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H144" s="77">
         <f t="shared" si="31"/>
         <v>2.7</v>
@@ -18811,7 +18811,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="146" spans="1:35">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.2">
       <c r="H146">
         <v>1</v>
       </c>
@@ -18897,7 +18897,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:35">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>281</v>
       </c>
@@ -19014,7 +19014,7 @@
         <v>22.700000000000003</v>
       </c>
     </row>
-    <row r="148" spans="1:35">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.2">
       <c r="H148" s="77">
         <f>H127+H141</f>
         <v>5.7</v>
@@ -19141,12 +19141,12 @@
       <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" thickBot="1">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
@@ -19211,7 +19211,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -19276,7 +19276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
@@ -19341,7 +19341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>111</v>
       </c>
@@ -19406,7 +19406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>108</v>
       </c>
@@ -19471,7 +19471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>110</v>
       </c>
@@ -19536,7 +19536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>109</v>
       </c>
@@ -19601,7 +19601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -19666,7 +19666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -19731,7 +19731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>114</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>113</v>
       </c>
@@ -19861,7 +19861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>112</v>
       </c>
@@ -19926,7 +19926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
@@ -19991,7 +19991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -20056,7 +20056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
@@ -20121,7 +20121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>107</v>
       </c>
@@ -20186,7 +20186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>103</v>
       </c>
@@ -20251,7 +20251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>104</v>
       </c>
@@ -20316,7 +20316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -20381,7 +20381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>105</v>
       </c>
@@ -20446,7 +20446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
@@ -20511,7 +20511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>42</v>
       </c>
@@ -20576,7 +20576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -20641,7 +20641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>118</v>
       </c>
@@ -20706,7 +20706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>117</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="16.5" thickBot="1">
+    <row r="26" spans="1:43" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>116</v>
       </c>
@@ -20836,7 +20836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
@@ -20860,7 +20860,7 @@
       <c r="AP27" s="4"/>
       <c r="AQ27" s="4"/>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
@@ -20884,7 +20884,7 @@
       <c r="AP28" s="4"/>
       <c r="AQ28" s="4"/>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -20907,7 +20907,7 @@
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -20930,7 +20930,7 @@
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -20953,7 +20953,7 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
     </row>
-    <row r="41" spans="1:27" ht="16.5" thickBot="1">
+    <row r="41" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="W41" t="s">
         <v>188</v>
       </c>
@@ -20961,7 +20961,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -21056,7 +21056,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -21151,7 +21151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -21246,7 +21246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -21341,7 +21341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -21436,7 +21436,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -21531,7 +21531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -21626,7 +21626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -21721,7 +21721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -21816,7 +21816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -21911,7 +21911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -22006,7 +22006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -22101,7 +22101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="15" customHeight="1">
+    <row r="54" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -22196,7 +22196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -22291,7 +22291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -22386,7 +22386,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -22481,7 +22481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -22576,7 +22576,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>106</v>
       </c>
@@ -22671,7 +22671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>105</v>
       </c>
@@ -22766,7 +22766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>34</v>
       </c>
@@ -22861,7 +22861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -22956,7 +22956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:27">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -23051,7 +23051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:27">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -23146,7 +23146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:60">
+    <row r="65" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -23241,7 +23241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:60" ht="16.5" thickBot="1">
+    <row r="66" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>116</v>
       </c>
@@ -23336,8 +23336,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:60" ht="16.5" thickBot="1"/>
-    <row r="68" spans="1:60" ht="16.5" thickBot="1">
+    <row r="67" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>190</v>
       </c>
@@ -23422,7 +23422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:60">
+    <row r="71" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>191</v>
       </c>
@@ -23508,7 +23508,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:60">
+    <row r="72" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>1</v>
       </c>
@@ -23678,7 +23678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="1:60">
+    <row r="73" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B73">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -23761,7 +23761,7 @@
       </c>
       <c r="AC73" s="69"/>
     </row>
-    <row r="74" spans="1:60">
+    <row r="74" spans="1:60" x14ac:dyDescent="0.2">
       <c r="C74">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -23844,7 +23844,7 @@
       </c>
       <c r="AC74" s="69"/>
     </row>
-    <row r="75" spans="1:60">
+    <row r="75" spans="1:60" x14ac:dyDescent="0.2">
       <c r="D75">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -23927,7 +23927,7 @@
       </c>
       <c r="AC75" s="69"/>
     </row>
-    <row r="76" spans="1:60">
+    <row r="76" spans="1:60" x14ac:dyDescent="0.2">
       <c r="E76">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24010,7 +24010,7 @@
       </c>
       <c r="AC76" s="69"/>
     </row>
-    <row r="77" spans="1:60">
+    <row r="77" spans="1:60" x14ac:dyDescent="0.2">
       <c r="F77">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24093,7 +24093,7 @@
       </c>
       <c r="AC77" s="69"/>
     </row>
-    <row r="78" spans="1:60">
+    <row r="78" spans="1:60" x14ac:dyDescent="0.2">
       <c r="I78">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24176,7 +24176,7 @@
       </c>
       <c r="AC78" s="69"/>
     </row>
-    <row r="79" spans="1:60">
+    <row r="79" spans="1:60" x14ac:dyDescent="0.2">
       <c r="J79">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24258,7 +24258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:60">
+    <row r="80" spans="1:60" x14ac:dyDescent="0.2">
       <c r="K80">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24340,7 +24340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:60">
+    <row r="81" spans="1:60" x14ac:dyDescent="0.2">
       <c r="L81">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24422,7 +24422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:60">
+    <row r="82" spans="1:60" x14ac:dyDescent="0.2">
       <c r="M82">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24504,7 +24504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:60">
+    <row r="83" spans="1:60" x14ac:dyDescent="0.2">
       <c r="P83">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24586,7 +24586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:60">
+    <row r="84" spans="1:60" x14ac:dyDescent="0.2">
       <c r="Q84">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24668,7 +24668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:60">
+    <row r="85" spans="1:60" x14ac:dyDescent="0.2">
       <c r="R85">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24750,7 +24750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:60">
+    <row r="86" spans="1:60" x14ac:dyDescent="0.2">
       <c r="S86">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24832,7 +24832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:60">
+    <row r="87" spans="1:60" x14ac:dyDescent="0.2">
       <c r="T87">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24914,7 +24914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:60">
+    <row r="88" spans="1:60" x14ac:dyDescent="0.2">
       <c r="W88">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -24996,7 +24996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:60">
+    <row r="89" spans="1:60" x14ac:dyDescent="0.2">
       <c r="X89">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -25078,7 +25078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:60">
+    <row r="90" spans="1:60" x14ac:dyDescent="0.2">
       <c r="Y90">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -25160,7 +25160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:60">
+    <row r="91" spans="1:60" x14ac:dyDescent="0.2">
       <c r="Z91">
         <f>$B$68</f>
         <v>3.1849598388794802</v>
@@ -25242,7 +25242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:60">
+    <row r="92" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B92" s="73"/>
       <c r="C92" s="73"/>
       <c r="D92" s="73"/>
@@ -25349,7 +25349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:60" ht="16.5" thickBot="1">
+    <row r="93" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>198</v>
       </c>
@@ -25466,7 +25466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:60" ht="16.5" thickBot="1">
+    <row r="94" spans="1:60" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AF94" t="s">
         <v>198</v>
       </c>
@@ -25575,7 +25575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:60">
+    <row r="95" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>281</v>
       </c>
@@ -25692,7 +25692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:60">
+    <row r="96" spans="1:60" x14ac:dyDescent="0.2">
       <c r="AF96" t="s">
         <v>201</v>
       </c>
@@ -25781,7 +25781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:60">
+    <row r="97" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>283</v>
       </c>
@@ -25985,7 +25985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:60">
+    <row r="98" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>282</v>
       </c>
@@ -26077,17 +26077,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:60">
+    <row r="99" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>5.5</v>
       </c>
     </row>
-    <row r="100" spans="1:60">
+    <row r="100" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:60">
+    <row r="102" spans="1:60" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
         <v>285</v>
       </c>
@@ -26101,7 +26101,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="103" spans="1:60">
+    <row r="103" spans="1:60" x14ac:dyDescent="0.2">
       <c r="C103" s="75">
         <f>(SUM(B97:E97)+SUM(I97:L97)+SUM(P97:S97)+SUM(W97:Z97))/(16)</f>
         <v>0.7985184567457424</v>
@@ -26118,7 +26118,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="107" spans="1:60">
+    <row r="107" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>290</v>
       </c>
@@ -26135,7 +26135,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="108" spans="1:60">
+    <row r="108" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>288</v>
       </c>
@@ -26155,7 +26155,7 @@
         <v>0.76121710071844428</v>
       </c>
     </row>
-    <row r="109" spans="1:60">
+    <row r="109" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>200</v>
       </c>
@@ -26175,7 +26175,7 @@
         <v>0.75812510778581255</v>
       </c>
     </row>
-    <row r="110" spans="1:60">
+    <row r="110" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>291</v>
       </c>
@@ -26208,10 +26208,10 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="16.5" thickBot="1"/>
-    <row r="2" spans="1:29">
+    <row r="1" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>299</v>
       </c>
@@ -26300,7 +26300,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="16.5" thickBot="1">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
         <v>5.5</v>
       </c>
@@ -26386,8 +26386,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="16.5" thickBot="1"/>
-    <row r="6" spans="1:29">
+    <row r="5" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>300</v>
       </c>
@@ -26476,7 +26476,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="16.5" thickBot="1">
+    <row r="7" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14">
         <v>11</v>
       </c>
@@ -26568,6 +26568,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010014502AD36FC4D1459EE8BFEB917118AE" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b4cd19ef6f825a6ac181b2aef79b604">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1a062c2-eeb0-45d1-8c80-71eb2bb91349" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="944c6668d3530cb8510fee0a023b67da" ns2:_="">
     <xsd:import namespace="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
@@ -26739,35 +26754,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26789,9 +26779,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>